<commit_message>
update of report of the results
</commit_message>
<xml_diff>
--- a/plots_results/results_of_models.xlsx
+++ b/plots_results/results_of_models.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/mac_data/2022coding_files/Summer_project/plots_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7B6AA1-21E3-0140-BA00-1B867F8FF36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234DD68C-80AE-B046-8C55-AEB384F77DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9340" yWindow="1060" windowWidth="23100" windowHeight="18020" activeTab="2" xr2:uid="{0EDD3916-4BDC-CB4B-BE61-1DA424A7BAD2}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="19660" activeTab="1" xr2:uid="{0EDD3916-4BDC-CB4B-BE61-1DA424A7BAD2}"/>
   </bookViews>
   <sheets>
     <sheet name="dann" sheetId="1" r:id="rId1"/>
-    <sheet name="ssl" sheetId="2" r:id="rId2"/>
-    <sheet name="pretrained  models" sheetId="3" r:id="rId3"/>
+    <sheet name="pretrained  models" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,32 +35,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
-  <si>
-    <t>models</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A-&gt;W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>W-&gt;A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>model type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Resnet18</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Alexnet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,15 +57,82 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>the number of classes masked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Train Loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Test Loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Architecture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>office31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maskRandom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dann</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-&gt;A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-&gt;W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W-&gt;D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DataSet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">A-&gt;D </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A-&gt;W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maskrandom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alexnet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resnet18</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,23 +497,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78DF8BC-7AA0-D049-BEDD-73A2E8291DBE}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A2" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>8.1050000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>8.984</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>52.79</v>
+      </c>
+      <c r="F6">
+        <v>43.79</v>
+      </c>
+      <c r="G6">
+        <v>33.47</v>
+      </c>
+      <c r="H6">
+        <v>86.13</v>
+      </c>
+      <c r="I6">
+        <v>31.15</v>
+      </c>
+      <c r="J6">
+        <v>94.61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>49.41</v>
+      </c>
+      <c r="F7">
+        <v>51.5</v>
+      </c>
+      <c r="G7">
+        <v>28.69</v>
+      </c>
+      <c r="H7">
+        <v>90.03</v>
+      </c>
+      <c r="I7">
+        <v>30.14</v>
+      </c>
+      <c r="J7">
+        <v>93.91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -473,136 +705,119 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE9F1DC-0072-5246-A9B9-78B40B73117E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AFC142-BA3C-BB48-99EE-0BFB85006CF5}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="C2">
+        <v>46.51</v>
+      </c>
+      <c r="D2">
+        <v>70.709999999999994</v>
+      </c>
+      <c r="E2">
+        <v>0.58550000000000002</v>
+      </c>
+      <c r="F2">
+        <v>3.0009999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>46.81</v>
+      </c>
+      <c r="D3">
+        <v>70.540000000000006</v>
+      </c>
+      <c r="E3">
+        <v>0.42120000000000002</v>
+      </c>
+      <c r="F3">
+        <v>2.9359999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>60.85</v>
+      </c>
+      <c r="D4">
+        <v>83.43</v>
+      </c>
+      <c r="E4">
+        <v>2.7640000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>2.2050000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>61.31</v>
+      </c>
+      <c r="D5">
+        <v>83.69</v>
+      </c>
+      <c r="E5">
+        <v>2.8580000000000001E-2</v>
+      </c>
+      <c r="F5">
+        <v>2.1749999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>